<commit_message>
Refresh tokens actually working
The refresh token is now able to refresh the access and refresh tokens.
</commit_message>
<xml_diff>
--- a/Generator/files/recipe/RecipeNames.xlsx
+++ b/Generator/files/recipe/RecipeNames.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Mondragon\POPBL\mubisofteco\Generation\files\recipe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Mondragon\POPBL\mubisofteco\Generator\files\recipe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE2154E-47B3-4F75-85D7-43BDC4E8E5E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6DF1D6-11CF-401B-B236-CA98B5D5D9E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -186,9 +186,6 @@
     <t>Roasted</t>
   </si>
   <si>
-    <t>Spannish</t>
-  </si>
-  <si>
     <t>Gratinned</t>
   </si>
   <si>
@@ -304,6 +301,9 @@
   </si>
   <si>
     <t>Betelana</t>
+  </si>
+  <si>
+    <t>Spanish</t>
   </si>
 </sst>
 </file>
@@ -657,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -716,7 +716,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
         <v>31</v>
@@ -796,7 +796,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
         <v>32</v>
@@ -836,7 +836,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D5" t="s">
         <v>32</v>
@@ -876,7 +876,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D6" t="s">
         <v>31</v>
@@ -916,7 +916,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D7" t="s">
         <v>31</v>
@@ -936,7 +936,7 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D8" t="s">
         <v>31</v>
@@ -956,7 +956,7 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D9" t="s">
         <v>31</v>
@@ -985,7 +985,7 @@
         <v>18</v>
       </c>
       <c r="F10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.3">
@@ -996,7 +996,7 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D11" t="s">
         <v>31</v>
@@ -1016,7 +1016,7 @@
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D12" t="s">
         <v>31</v>
@@ -1036,7 +1036,7 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D13" t="s">
         <v>31</v>
@@ -1056,7 +1056,7 @@
         <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D14" t="s">
         <v>31</v>
@@ -1076,7 +1076,7 @@
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D15" t="s">
         <v>36</v>
@@ -1085,7 +1085,7 @@
         <v>18</v>
       </c>
       <c r="F15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.3">
@@ -1110,13 +1110,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17" t="s">
         <v>43</v>
       </c>
       <c r="C17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D17" t="s">
         <v>31</v>
@@ -1133,10 +1133,10 @@
         <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D18" t="s">
         <v>32</v>
@@ -1153,10 +1153,10 @@
         <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D19" t="s">
         <v>32</v>
@@ -1176,7 +1176,7 @@
         <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D20" t="s">
         <v>36</v>
@@ -1196,7 +1196,7 @@
         <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D21" t="s">
         <v>31</v>
@@ -1213,10 +1213,10 @@
         <v>48</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D22" t="s">
         <v>32</v>
@@ -1233,10 +1233,10 @@
         <v>49</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D23" t="s">
         <v>32</v>
@@ -1253,10 +1253,10 @@
         <v>50</v>
       </c>
       <c r="B24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D24" t="s">
         <v>32</v>
@@ -1273,10 +1273,10 @@
         <v>51</v>
       </c>
       <c r="B25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D25" t="s">
         <v>36</v>
@@ -1293,10 +1293,10 @@
         <v>52</v>
       </c>
       <c r="B26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D26" t="s">
         <v>32</v>
@@ -1310,13 +1310,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>53</v>
+        <v>92</v>
       </c>
       <c r="B27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D27" t="s">
         <v>32</v>
@@ -1330,13 +1330,13 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D28" t="s">
         <v>32</v>
@@ -1356,7 +1356,7 @@
         <v>24</v>
       </c>
       <c r="C29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1370,13 +1370,13 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B30" t="s">
         <v>42</v>
       </c>
       <c r="C30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D30" t="s">
         <v>31</v>

</xml_diff>